<commit_message>
fix python + excel kind of first day patch
</commit_message>
<xml_diff>
--- a/lab/02/Python/data.xlsx
+++ b/lab/02/Python/data.xlsx
@@ -19,7 +19,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="25">
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Prise</t>
+  </si>
+  <si>
+    <t>7A6D8AA2AC22A6B3C27D4B17536E2225D06E698D597D44F9C2BE07B927FC7BA6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">печенье </t>
+  </si>
+  <si>
+    <t>100 р</t>
+  </si>
+  <si>
+    <t xml:space="preserve">чай </t>
+  </si>
+  <si>
+    <t xml:space="preserve">мармеладные мишки </t>
+  </si>
+  <si>
+    <t>156 р</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кофие </t>
+  </si>
+  <si>
+    <t>200 р</t>
+  </si>
+  <si>
+    <t>ноутбук 1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rtx </t>
+  </si>
+  <si>
+    <t>несметные богатства</t>
+  </si>
+  <si>
+    <t xml:space="preserve">что то за </t>
+  </si>
+  <si>
+    <t>кого то</t>
+  </si>
+  <si>
+    <t>автомат пж</t>
+  </si>
+  <si>
+    <t xml:space="preserve">может </t>
+  </si>
+  <si>
+    <t>не надо</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ладно </t>
+  </si>
+  <si>
+    <t>хоть это</t>
+  </si>
+  <si>
+    <t xml:space="preserve">слитки золота </t>
+  </si>
+  <si>
+    <t>200000 шекелей</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,16 +437,396 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="A1:H11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="1"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44185.015217501437</v>
+      </c>
+      <c r="D12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="E17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="E20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44185.015235798797</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>